<commit_message>
Cleaner genus component project extension build
</commit_message>
<xml_diff>
--- a/tabular/genus/amdo-refseqs-side-data.xlsx
+++ b/tabular/genus/amdo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0523B37-F9FC-BF49-98CB-EBF8A975452F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ADD1E2-974C-104E-8080-DB982D063A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{469403FE-80B6-3840-B15B-8B62EF5C2974}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t xml:space="preserve"> Carnivore amdoparvovirus 1</t>
   </si>
@@ -50,9 +50,6 @@
     <t>ADV</t>
   </si>
   <si>
-    <t xml:space="preserve"> Carnivore amdoparvovirus 2</t>
-  </si>
-  <si>
     <t>gray fox amdovirus</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>GFAV</t>
   </si>
   <si>
-    <t xml:space="preserve"> Carnivore amdoparvovirus 3</t>
-  </si>
-  <si>
     <t>racoon dog and fox amdoparvovirus</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>RFAV</t>
   </si>
   <si>
-    <t xml:space="preserve"> Carnivore amdoparvovirus 4</t>
-  </si>
-  <si>
     <t>skunk amdoparvovirus</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>SKAV</t>
   </si>
   <si>
-    <t xml:space="preserve"> Carnivore amdoparvovirus 5</t>
-  </si>
-  <si>
     <t>red panda amdoparvovirus</t>
   </si>
   <si>
@@ -153,13 +141,25 @@
   </si>
   <si>
     <t>accession-other</t>
+  </si>
+  <si>
+    <t>MT770848</t>
+  </si>
+  <si>
+    <t>Labrador-amdoparvovirus-1</t>
+  </si>
+  <si>
+    <t>MULL</t>
+  </si>
+  <si>
+    <t>LAPV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +171,12 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -522,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5CE6FC-94FB-E64A-8308-5869E9818659}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="E22:F22"/>
+      <selection activeCell="E5" sqref="A1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,46 +543,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -593,31 +599,31 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N2" t="s">
         <v>2</v>
@@ -625,181 +631,226 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added novel AmdoPV taxa
</commit_message>
<xml_diff>
--- a/tabular/genus/amdo-refseqs-side-data.xlsx
+++ b/tabular/genus/amdo-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvovirus-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNA/Parvovirus-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181DD8CE-41EA-D84F-A049-209B7A87A2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9027AA-B22A-DE49-9D33-E08045664FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3800" windowWidth="28040" windowHeight="17440" xr2:uid="{469403FE-80B6-3840-B15B-8B62EF5C2974}"/>
+    <workbookView xWindow="18480" yWindow="7440" windowWidth="28040" windowHeight="17440" xr2:uid="{469403FE-80B6-3840-B15B-8B62EF5C2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t xml:space="preserve"> Carnivore amdoparvovirus 1</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Labrador-amdoparvovirus-1</t>
   </si>
   <si>
-    <t>MULL</t>
-  </si>
-  <si>
-    <t>LAPV</t>
-  </si>
-  <si>
     <t>Urocyon cinereoargenteus</t>
   </si>
   <si>
@@ -180,6 +174,51 @@
   </si>
   <si>
     <t>sequenceID</t>
+  </si>
+  <si>
+    <t>KJ641663</t>
+  </si>
+  <si>
+    <t>KY432922</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carnivore amdoparvovirus 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carnivore amdoparvovirus 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carnivore amdoparvovirus 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carnivore amdoparvovirus 5</t>
+  </si>
+  <si>
+    <t>LaAV-1</t>
+  </si>
+  <si>
+    <t>RtRn-ParV</t>
+  </si>
+  <si>
+    <t>BtRl-PV</t>
+  </si>
+  <si>
+    <t>Rattus nitidus parvovirus</t>
+  </si>
+  <si>
+    <t>Rhinolophus lepidus parvovirus</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Rhinolophus lepidus</t>
+  </si>
+  <si>
+    <t>Rattus nitidus</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -555,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5CE6FC-94FB-E64A-8308-5869E9818659}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,13 +611,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>22</v>
@@ -625,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -634,10 +673,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -672,19 +711,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -719,19 +758,19 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -766,19 +805,19 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -813,19 +852,19 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -857,46 +896,140 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor build and phylogeny
</commit_message>
<xml_diff>
--- a/tabular/genus/amdo-refseqs-side-data.xlsx
+++ b/tabular/genus/amdo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNA/Parvovirus-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9027AA-B22A-DE49-9D33-E08045664FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB15522-4919-2E4C-9FD6-F23DAC51F9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18480" yWindow="7440" windowWidth="28040" windowHeight="17440" xr2:uid="{469403FE-80B6-3840-B15B-8B62EF5C2974}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,19 +943,19 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
         <v>41</v>
@@ -990,19 +990,19 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
         <v>41</v>

</xml_diff>